<commit_message>
mas graficos en plantas
</commit_message>
<xml_diff>
--- a/CMPC_Manufacturing/InputCMPC.xlsx
+++ b/CMPC_Manufacturing/InputCMPC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ite02\Documents\Gaston\Source\CMPC-manufacturing\CMCP_Manufacturing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ite02\Documents\Gaston\Source\CMPC-manufacturing\CMPC_Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C2AE00-DB48-4A22-83A8-05DCF98E84EE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BB1304-D2C3-4F14-B383-6A5ACA70F551}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17940" windowHeight="6045" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="109">
   <si>
     <t>sku</t>
   </si>
@@ -1652,10 +1652,10 @@
   <dimension ref="A1:R277"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="I264" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A248" activeCellId="3" sqref="A49 A127 A196 A248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -17204,15 +17204,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A8B674-5D45-452C-8160-27DDD23798C3}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="1" max="1" width="26.25" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17235,7 +17235,7 @@
         <v>80</v>
       </c>
       <c r="C2" s="1">
-        <v>300</v>
+        <v>800</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -17247,6 +17247,50 @@
       </c>
       <c r="C3" s="1">
         <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="1">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="1">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="1">
+        <v>800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
demanda y no real_demand. correccion en el output de sku
</commit_message>
<xml_diff>
--- a/CMPC_Manufacturing/InputCMPC.xlsx
+++ b/CMPC_Manufacturing/InputCMPC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ite02\Documents\Gaston\Source\CMPC-manufacturing\CMPC_Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BB1304-D2C3-4F14-B383-6A5ACA70F551}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029FD2A1-2A69-4EC1-8E01-79ADBC39FC35}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17940" windowHeight="6045" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17940" windowHeight="6045" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SKU" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="109">
   <si>
     <t>sku</t>
   </si>
@@ -438,7 +438,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -449,6 +449,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -881,7 +887,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -893,6 +899,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="283" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="418">
     <cellStyle name="60% - Accent1 2" xfId="351" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -17206,8 +17213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A8B674-5D45-452C-8160-27DDD23798C3}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17217,13 +17224,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="11" t="s">
         <v>106</v>
       </c>
     </row>
@@ -18430,10 +18437,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:O1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -18452,7 +18459,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
@@ -19474,6 +19481,47 @@
       </c>
       <c r="M25">
         <v>3.9999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="7">
+        <v>450</v>
+      </c>
+      <c r="C26" s="7">
+        <v>7</v>
+      </c>
+      <c r="D26" s="7">
+        <v>2</v>
+      </c>
+      <c r="E26" s="7">
+        <v>9</v>
+      </c>
+      <c r="F26" s="7">
+        <v>49.620932307692293</v>
+      </c>
+      <c r="G26" s="7">
+        <v>2.8</v>
+      </c>
+      <c r="H26" s="7">
+        <v>73.3</v>
+      </c>
+      <c r="I26" s="7">
+        <v>81.478548846153828</v>
+      </c>
+      <c r="J26" s="7">
+        <v>287.3</v>
+      </c>
+      <c r="K26" s="7">
+        <v>9406</v>
+      </c>
+      <c r="L26" s="7">
+        <v>1456</v>
+      </c>
+      <c r="M26" s="7">
+        <v>-0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>